<commit_message>
Updated for fall 2022
Partially updated
</commit_message>
<xml_diff>
--- a/LabStarters/Lab03/Lab3Rubric-CIS195.xlsx
+++ b/LabStarters/Lab03/Lab3Rubric-CIS195.xlsx
@@ -1,25 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CIS195-CourseMaterials/LabStarters/Lab03/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Repos\CIS195-CourseMaterials\LabStarters\Lab03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC96058-F2B8-7D4A-94E9-ADCC94CD0A3D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57ABA9D-197E-4FC1-84E2-E1A9C9DDF26A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="460" windowWidth="10880" windowHeight="14780" activeTab="1" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
+    <workbookView xWindow="40680" yWindow="-2688" windowWidth="13044" windowHeight="13752" activeTab="1" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -91,9 +100,6 @@
     <t>Part 1: Internal links</t>
   </si>
   <si>
-    <t>nav</t>
-  </si>
-  <si>
     <t>image links</t>
   </si>
   <si>
@@ -122,6 +128,9 @@
   </si>
   <si>
     <t>Part 2: Image Map</t>
+  </si>
+  <si>
+    <t>nav element with links</t>
   </si>
 </sst>
 </file>
@@ -506,17 +515,17 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -527,7 +536,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -538,7 +547,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -549,7 +558,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -560,7 +569,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -571,7 +580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -582,7 +591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -593,7 +602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -604,7 +613,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -615,7 +624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
@@ -628,12 +637,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
@@ -644,7 +653,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -655,7 +664,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -666,7 +675,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -677,7 +686,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -688,7 +697,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -699,7 +708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -710,7 +719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -721,7 +730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>17</v>
       </c>
@@ -744,20 +753,23 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.19921875" customWidth="1"/>
+    <col min="2" max="2" width="6.19921875" customWidth="1"/>
+    <col min="3" max="3" width="7.59765625" customWidth="1"/>
+    <col min="4" max="4" width="11.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -768,9 +780,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -779,9 +791,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>8</v>
@@ -790,21 +802,21 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>23</v>
-      </c>
       <c r="B6">
         <v>4</v>
       </c>
@@ -812,7 +824,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
@@ -825,12 +837,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -841,9 +853,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11">
         <v>2</v>
@@ -852,9 +864,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12">
         <v>9</v>
@@ -863,9 +875,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -874,9 +886,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14">
         <v>9</v>
@@ -885,9 +897,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15">
         <v>3</v>
@@ -896,9 +908,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2">
         <v>3</v>
@@ -907,7 +919,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
@@ -922,5 +934,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added the rubric to the instructions
</commit_message>
<xml_diff>
--- a/LabStarters/Lab03/Lab3Rubric-CIS195.xlsx
+++ b/LabStarters/Lab03/Lab3Rubric-CIS195.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Repos\CIS195-CourseMaterials\LabStarters\Lab03\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Documents\GitHub\CIS195-CourseMaterials\LabStarters\Lab03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57ABA9D-197E-4FC1-84E2-E1A9C9DDF26A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3CAECB-FE6B-48B2-A20A-6C5029BD0CC9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40680" yWindow="-2688" windowWidth="13044" windowHeight="13752" activeTab="1" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
+    <workbookView xWindow="40680" yWindow="-2685" windowWidth="13050" windowHeight="13755" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Rubric" sheetId="1" r:id="rId1"/>
+    <sheet name="Grade" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -511,21 +511,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7896AEF-34AA-E746-914C-B3A1A695E7D1}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -536,7 +536,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -547,7 +547,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -558,7 +558,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -569,7 +569,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -580,7 +580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -591,7 +591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -602,7 +602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -613,7 +613,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -624,7 +624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
@@ -637,12 +637,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
@@ -653,7 +653,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -664,7 +664,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -675,7 +675,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -686,7 +686,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -697,7 +697,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -708,7 +708,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -719,7 +719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -730,7 +730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>17</v>
       </c>
@@ -745,6 +745,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <webPublishItems count="1">
+    <webPublishItem id="90" divId="Lab3Rubric-CIS195_90" sourceType="sheet" destinationFile="C:\Users\Student\Documents\GitHub\CIS195-CourseMaterials\LabStarters\Lab03\Lab3Rubric-CIS195.htm"/>
+  </webPublishItems>
 </worksheet>
 </file>
 
@@ -752,24 +755,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96879333-0874-3847-ABBB-D0DF183A7724}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.19921875" customWidth="1"/>
-    <col min="2" max="2" width="6.19921875" customWidth="1"/>
-    <col min="3" max="3" width="7.59765625" customWidth="1"/>
-    <col min="4" max="4" width="11.19921875" customWidth="1"/>
+    <col min="1" max="1" width="20.25" customWidth="1"/>
+    <col min="2" max="2" width="6.25" customWidth="1"/>
+    <col min="3" max="3" width="7.625" customWidth="1"/>
+    <col min="4" max="4" width="11.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -780,7 +783,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -791,7 +794,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -802,7 +805,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -813,7 +816,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -824,7 +827,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
@@ -837,12 +840,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
@@ -853,7 +856,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -864,7 +867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -875,7 +878,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -886,7 +889,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -897,7 +900,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -908,7 +911,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -919,7 +922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
added date to grading page
</commit_message>
<xml_diff>
--- a/LabStarters/Lab03/Lab3Rubric-CIS195.xlsx
+++ b/LabStarters/Lab03/Lab3Rubric-CIS195.xlsx
@@ -1,34 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\CIS195-CourseMaterials\LabStarters\Lab03\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CIS195-CourseMaterials/LabStarters/Lab03/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC361727-6742-4E6A-85BF-E1E278983A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA8E9F0-672A-E445-8881-2F2F35F18BE0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32256" yWindow="4188" windowWidth="15900" windowHeight="15576" activeTab="1" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
+    <workbookView xWindow="9700" yWindow="500" windowWidth="15900" windowHeight="14640" activeTab="1" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
     <sheet name="Grade" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -139,7 +130,7 @@
     <t>Style, syntax and format</t>
   </si>
   <si>
-    <t>Lab 3</t>
+    <t>Here's the grade breakdown:</t>
   </si>
 </sst>
 </file>
@@ -199,12 +190,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,17 +520,17 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -544,7 +539,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -552,7 +547,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -560,7 +555,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -568,7 +563,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -576,7 +571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -584,7 +579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -593,7 +588,7 @@
       </c>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -602,7 +597,7 @@
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -611,7 +606,7 @@
       </c>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
@@ -621,12 +616,12 @@
       </c>
       <c r="C11" s="3"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
@@ -635,7 +630,7 @@
       </c>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -643,7 +638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -651,7 +646,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -659,7 +654,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -667,7 +662,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -676,7 +671,7 @@
       </c>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -685,7 +680,7 @@
       </c>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -694,7 +689,7 @@
       </c>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>17</v>
       </c>
@@ -714,232 +709,239 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96879333-0874-3847-ABBB-D0DF183A7724}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.59765625" customWidth="1"/>
-    <col min="2" max="2" width="6.19921875" customWidth="1"/>
-    <col min="3" max="3" width="7.59765625" customWidth="1"/>
-    <col min="4" max="4" width="11.19921875" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>30</v>
       </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>22</v>
       </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>31</v>
       </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>21</v>
       </c>
-      <c r="B7">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="3">
-        <f>SUM(B4:B7)</f>
+      <c r="B9" s="3">
+        <f>SUM(B5:B8)</f>
         <v>16</v>
       </c>
-      <c r="C8" s="3">
-        <f>SUM(C4:C7)</f>
+      <c r="C9" s="3">
+        <f>SUM(C5:C8)</f>
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>2</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>24</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>9</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>25</v>
       </c>
-      <c r="B14">
-        <v>4</v>
-      </c>
-      <c r="C14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>27</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>6</v>
       </c>
-      <c r="C15">
+      <c r="C16">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>32</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <v>3</v>
       </c>
-      <c r="C16">
+      <c r="C17">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B18" s="4">
         <v>3</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C18" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="3">
-        <f>SUM(B12:B17)</f>
+      <c r="B19" s="3">
+        <f>SUM(B13:B18)</f>
         <v>27</v>
       </c>
-      <c r="C18" s="3">
-        <f>SUM(C12:C17)</f>
+      <c r="C19" s="3">
+        <f>SUM(C13:C18)</f>
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B21" s="3">
         <v>7</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C21" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="1">
-        <f>B8+B18+B20</f>
+      <c r="B23" s="1">
+        <f>B9+B19+B21</f>
         <v>50</v>
       </c>
-      <c r="C22" s="1">
-        <f>C8+C18+C20</f>
+      <c r="C23" s="1">
+        <f>C9+C19+C21</f>
         <v>50</v>
       </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="6">
+        <f ca="1">NOW()</f>
+        <v>44856.439880208331</v>
+      </c>
+      <c r="B24" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <webPublishItems count="1">
-    <webPublishItem id="30539" divId="Lab3Rubric-CIS195_30539" sourceType="range" sourceRef="A1:C22" destinationFile="D:\Repos\CIS195-CourseMaterials\LabStarters\Lab03\Lab3Rubric-CIS195.htm"/>
+    <webPublishItem id="30539" divId="Lab3Rubric-CIS195_30539" sourceType="range" sourceRef="A1:C23" destinationFile="D:\Repos\CIS195-CourseMaterials\LabStarters\Lab03\Lab3Rubric-CIS195.htm"/>
   </webPublishItems>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated and clarified the lab assignments
</commit_message>
<xml_diff>
--- a/LabStarters/Lab03/Lab3Rubric-CIS195.xlsx
+++ b/LabStarters/Lab03/Lab3Rubric-CIS195.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CIS195-CourseMaterials/LabStarters/Lab03/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA8E9F0-672A-E445-8881-2F2F35F18BE0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF0EC86-4A03-4849-A66E-EF97672D0D54}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9700" yWindow="500" windowWidth="15900" windowHeight="14640" activeTab="1" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
+    <workbookView xWindow="9700" yWindow="500" windowWidth="15900" windowHeight="14620" activeTab="1" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubric" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>Elements used:</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>Here's the grade breakdown:</t>
+  </si>
+  <si>
+    <t>Not used</t>
   </si>
 </sst>
 </file>
@@ -190,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -200,6 +203,7 @@
     <xf numFmtId="22" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -709,10 +713,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96879333-0874-3847-ABBB-D0DF183A7724}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -724,9 +728,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>34</v>
       </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -861,7 +867,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -872,7 +878,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -880,10 +886,13 @@
         <v>3</v>
       </c>
       <c r="C18" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>29</v>
       </c>
@@ -893,15 +902,15 @@
       </c>
       <c r="C19" s="3">
         <f>SUM(C13:C18)</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>33</v>
       </c>
@@ -912,12 +921,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
@@ -927,17 +936,20 @@
       </c>
       <c r="C23" s="1">
         <f>C9+C19+C21</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <f ca="1">NOW()</f>
-        <v>44856.439880208331</v>
+        <v>44856.564592592593</v>
       </c>
       <c r="B24" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <webPublishItems count="1">

</xml_diff>

<commit_message>
Updates to syllabus, revisions to rubrics
</commit_message>
<xml_diff>
--- a/LabStarters/Lab03/Lab3Rubric-CIS195.xlsx
+++ b/LabStarters/Lab03/Lab3Rubric-CIS195.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CIS195-CourseMaterials/LabStarters/Lab03/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF0EC86-4A03-4849-A66E-EF97672D0D54}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35E5EC3-7A18-864D-A944-50AD8E6260BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9700" yWindow="500" windowWidth="15900" windowHeight="14620" activeTab="1" xr2:uid="{5D75B731-65CD-014E-8BBA-DE69945DF98D}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
   <si>
     <t>Elements used:</t>
   </si>
@@ -131,9 +131,6 @@
   </si>
   <si>
     <t>Here's the grade breakdown:</t>
-  </si>
-  <si>
-    <t>Not used</t>
   </si>
 </sst>
 </file>
@@ -713,10 +710,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96879333-0874-3847-ABBB-D0DF183A7724}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -867,7 +864,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -878,7 +875,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -886,13 +883,10 @@
         <v>3</v>
       </c>
       <c r="C18" s="4">
-        <v>0</v>
-      </c>
-      <c r="D18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>29</v>
       </c>
@@ -902,15 +896,15 @@
       </c>
       <c r="C19" s="3">
         <f>SUM(C13:C18)</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>33</v>
       </c>
@@ -921,12 +915,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>17</v>
       </c>
@@ -936,13 +930,13 @@
       </c>
       <c r="C23" s="1">
         <f>C9+C19+C21</f>
-        <v>47</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <f ca="1">NOW()</f>
-        <v>44856.564592592593</v>
+        <v>44881.596260995371</v>
       </c>
       <c r="B24" s="5"/>
     </row>

</xml_diff>